<commit_message>
Massor av ändringar efter arbete för telenor
</commit_message>
<xml_diff>
--- a/SiteCrawler/ResultExcelTemplate.xlsx
+++ b/SiteCrawler/ResultExcelTemplate.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tests!$A$4:$E$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tests!$A$6:$F$6</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Status</t>
   </si>
@@ -44,13 +44,28 @@
   </si>
   <si>
     <t>Target</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Invalid Colors</t>
+  </si>
+  <si>
+    <t>Invalid Icons</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,6 +83,15 @@
     </font>
     <font>
       <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -127,17 +151,46 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="10" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -188,7 +241,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -230,7 +283,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -263,26 +316,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -315,23 +351,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -507,95 +526,140 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.265625" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="10.1328125" customWidth="1"/>
-    <col min="5" max="7" width="33.59765625" customWidth="1"/>
+    <col min="1" max="1" width="60.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="64.5703125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="67.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="E1" s="1" t="s">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="8">
+        <f>SUM(C2:C4)</f>
+        <v>0</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="e">
+        <f>C2/C1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="C2" s="8">
+        <f>COUNTIF(B7:B10000,"Passed")</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="e">
+        <f>C3/C1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="C3" s="8">
+        <f>COUNTIF(B7:B10000,"Failed")</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="e">
+        <f>C4/C1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="C4" s="8">
+        <f>COUNTIF(B7:B10000,"Inconclusive")</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
     </row>
-    <row r="2" spans="1:8" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="E2" s="2" t="e">
-        <f>E3/H3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F2" s="3" t="e">
-        <f>F3/H3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G2" s="4" t="e">
-        <f>G3/H3</f>
-        <v>#DIV/0!</v>
-      </c>
+    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E3">
-        <f>COUNTIF(B5:B9998,"Passed")</f>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F3">
-        <f>COUNTIF(B5:B9998,"Fail")</f>
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <f>COUNTIF(B5:B9998,"Inconclusive")</f>
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <f>SUM(E3:G3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:E4" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="B4:B1048576">
+  <autoFilter ref="A6:F6"/>
+  <conditionalFormatting sqref="B6:B1048576">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Inconclusive"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"Fail"</formula>
+      <formula>"Failed"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Passed"</formula>

</xml_diff>

<commit_message>
- Brytit ut tester till separata filer - Lagt till TestResults property till Page
</commit_message>
<xml_diff>
--- a/SiteCrawler/ResultExcelTemplate.xlsx
+++ b/SiteCrawler/ResultExcelTemplate.xlsx
@@ -17,10 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Status</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Passed</t>
   </si>
@@ -34,12 +31,6 @@
     <t>Inconclusive</t>
   </si>
   <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>Duration</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -49,16 +40,16 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Invalid Colors</t>
-  </si>
-  <si>
-    <t>Invalid Icons</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Comment</t>
   </si>
 </sst>
 </file>
@@ -151,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -180,14 +171,8 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -241,7 +226,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -527,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,67 +526,55 @@
     <col min="4" max="4" width="13.7109375" style="6" customWidth="1"/>
     <col min="5" max="5" width="64.5703125" style="6" customWidth="1"/>
     <col min="6" max="6" width="67.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="22.85546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="13" t="s">
-        <v>3</v>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="11" t="s">
+        <v>2</v>
       </c>
       <c r="C1" s="8">
         <f>SUM(C2:C4)</f>
         <v>0</v>
       </c>
       <c r="F1" s="2"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="e">
         <f>C2/C1</f>
         <v>#DIV/0!</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="8">
         <f>COUNTIF(B7:B10000,"Passed")</f>
         <v>0</v>
       </c>
       <c r="F2" s="2"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="e">
         <f>C3/C1</f>
         <v>#DIV/0!</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="8">
         <f>COUNTIF(B7:B10000,"Failed")</f>
         <v>0</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="e">
         <f>C4/C1</f>
         <v>#DIV/0!</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="8">
         <f>COUNTIF(B7:B10000,"Inconclusive")</f>
@@ -609,47 +582,32 @@
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
     </row>
-    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>7</v>
+      <c r="G6" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>